<commit_message>
GDPR - Changes to the template
</commit_message>
<xml_diff>
--- a/template RGPD registos.xlsx
+++ b/template RGPD registos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="123" documentId="114_{4FC6CB05-B107-4692-B77D-C0EBC8DE0B3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0EC878DE-EF40-4BD3-B227-AC630B6F9764}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956C25C9-4560-4D05-8050-855A188EFC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="histórico de alterações" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="418">
   <si>
     <t>Nome</t>
   </si>
@@ -1219,15 +1219,6 @@
     <t xml:space="preserve">Consentimento; Contrato; </t>
   </si>
   <si>
-    <t xml:space="preserve">Consentimento; Interesse do Titular </t>
-  </si>
-  <si>
-    <t>Consentimento; Interesse do Titular; Interesse Público</t>
-  </si>
-  <si>
-    <t>Consentimento; Interesse do Responsável; Interesse do Titular</t>
-  </si>
-  <si>
     <t>1,2</t>
   </si>
   <si>
@@ -1240,9 +1231,6 @@
     <t>Localidade para correspondência e intendimento da localização do cliente</t>
   </si>
   <si>
-    <t>Empresa de Transporte</t>
-  </si>
-  <si>
     <t>223 483 707</t>
   </si>
   <si>
@@ -1292,6 +1280,18 @@
   </si>
   <si>
     <t>opt@hotmail.com</t>
+  </si>
+  <si>
+    <t>Empresa de Transporte LDA</t>
+  </si>
+  <si>
+    <t>Consentimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controlar a maioridade e adaptar escalão </t>
+  </si>
+  <si>
+    <t>Idade</t>
   </si>
 </sst>
 </file>
@@ -1563,10 +1563,40 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1577,21 +1607,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1631,21 +1646,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2032,17 +2032,17 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="56">
+      <c r="A3" s="33">
         <v>44170</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,8 +2314,8 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,28 +2326,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="11" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="40"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2385,41 +2385,41 @@
         <v>353</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="57" t="s">
-        <v>405</v>
+      <c r="B8" s="41"/>
+      <c r="C8" s="34" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="58">
+      <c r="B9" s="41"/>
+      <c r="C9" s="35">
         <v>279045668</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="31"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="5" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2448,7 +2448,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2457,50 +2457,50 @@
         <v>353</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="59" t="s">
-        <v>410</v>
+      <c r="B16" s="44"/>
+      <c r="C16" s="36" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="60">
+      <c r="B17" s="44"/>
+      <c r="C17" s="37">
         <v>920145789</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="38" t="s">
         <v>371</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="32"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="11" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="11" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2511,7 +2511,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2520,7 +2520,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2538,34 +2538,29 @@
         <v>353</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="57" t="s">
-        <v>417</v>
+      <c r="B25" s="41"/>
+      <c r="C25" s="34" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="58">
+      <c r="B26" s="41"/>
+      <c r="C26" s="35">
         <v>279466554</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:C10"/>
@@ -2575,6 +2570,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1" xr:uid="{04D58837-3C77-46B1-96CD-90ECA1153F10}"/>
@@ -2598,12 +2598,12 @@
   </sheetPr>
   <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:C2"/>
       <selection pane="topRight" sqref="A1:C2"/>
       <selection pane="bottomLeft" sqref="A1:C2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2616,77 +2616,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="42" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="49" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="53" t="s">
         <v>373</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="53" t="s">
         <v>372</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="53" t="s">
         <v>375</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="53" t="s">
         <v>376</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="53" t="s">
         <v>377</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="53" t="s">
         <v>379</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="L2" s="46" t="s">
+      <c r="L2" s="53" t="s">
         <v>381</v>
       </c>
-      <c r="M2" s="42"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="42"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="49"/>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
@@ -2695,11 +2695,11 @@
       <c r="B4" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -2716,16 +2716,16 @@
         <v>17</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>399</v>
-      </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+        <v>396</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
-      <c r="I5" s="54" t="s">
-        <v>398</v>
+      <c r="I5" s="31" t="s">
+        <v>395</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -2741,9 +2741,9 @@
       <c r="B6" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="54" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="31" t="s">
         <v>383</v>
       </c>
       <c r="F6" s="25"/>
@@ -2754,7 +2754,7 @@
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
       <c r="M6" s="25" t="s">
-        <v>394</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
         <v>386</v>
       </c>
       <c r="C7" s="25"/>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="31" t="s">
         <v>382</v>
       </c>
       <c r="E7" s="25"/>
@@ -2777,7 +2777,7 @@
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
       <c r="M7" s="25" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
         <v>386</v>
       </c>
       <c r="C8" s="25"/>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="31" t="s">
         <v>384</v>
       </c>
       <c r="E8" s="25"/>
@@ -2800,7 +2800,7 @@
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
       <c r="M8" s="25" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -2813,7 +2813,7 @@
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="31" t="s">
         <v>387</v>
       </c>
       <c r="G9" s="25"/>
@@ -2823,7 +2823,7 @@
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
       <c r="M9" s="25" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -2846,15 +2846,19 @@
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
       <c r="M10" s="22" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>417</v>
+      </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
@@ -2864,7 +2868,9 @@
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
+      <c r="M11" s="22" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
@@ -4520,24 +4526,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="49" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="56" t="s">
         <v>356</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="56" t="s">
         <v>358</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="53" t="s">
         <v>360</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="53" t="s">
         <v>352</v>
       </c>
       <c r="I1" s="4"/>
@@ -4551,7 +4557,7 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
+      <c r="A2" s="55"/>
       <c r="B2" s="27" t="s">
         <v>355</v>
       </c>
@@ -4561,10 +4567,10 @@
       <c r="D2" s="27" t="s">
         <v>359</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>

</xml_diff>

<commit_message>
C.14. Privacy Policy complete
</commit_message>
<xml_diff>
--- a/template RGPD registos.xlsx
+++ b/template RGPD registos.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956C25C9-4560-4D05-8050-855A188EFC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{956C25C9-4560-4D05-8050-855A188EFC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{491BA31B-9D70-4ABB-AB91-E0FA5BA96973}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1485" yWindow="1470" windowWidth="15300" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="histórico de alterações" sheetId="9" r:id="rId1"/>
@@ -1578,25 +1578,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1607,6 +1592,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2314,8 +2314,8 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,26 +2326,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="11" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="43"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="11" t="s">
         <v>397</v>
       </c>
@@ -2389,35 +2389,35 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="41"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="34" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="41"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="35">
         <v>279045668</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="44"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="5" t="s">
         <v>402</v>
       </c>
@@ -2461,44 +2461,44 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="44"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="36" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="37">
         <v>920145789</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="11" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="B20" s="43"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="11" t="s">
         <v>408</v>
       </c>
@@ -2542,25 +2542,30 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="41"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="34" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="41"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="35">
         <v>279466554</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:C10"/>
@@ -2570,11 +2575,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1" xr:uid="{04D58837-3C77-46B1-96CD-90ECA1153F10}"/>
@@ -2598,8 +2598,8 @@
   </sheetPr>
   <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:C2"/>
       <selection pane="topRight" sqref="A1:C2"/>
       <selection pane="bottomLeft" sqref="A1:C2"/>

</xml_diff>